<commit_message>
added validation error comments to adv-distribution-good.xlsx and completed adv-shipping-pandas.ipynb
</commit_message>
<xml_diff>
--- a/excel/adv-distribution-goods.xlsx
+++ b/excel/adv-distribution-goods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejwda\Google Drive\01-ejw-data-github\Public\Algorithms\algo-linear-programming\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA395C0-FEA3-4957-8D19-4E2319461835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E48B90-4864-496A-B74F-91B2628F6C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="690" windowWidth="28830" windowHeight="15510" activeTab="1" xr2:uid="{892D736E-9111-411A-81B5-8617378C0CEA}"/>
+    <workbookView xWindow="-28920" yWindow="1170" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{892D736E-9111-411A-81B5-8617378C0CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Starter_Template" sheetId="2" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="103">
   <si>
     <t>Beds</t>
   </si>
@@ -400,13 +400,25 @@
   </si>
   <si>
     <t>Yellow Tables are variables that can be changed by the solver and the contents can be deleted prior to running the solver</t>
+  </si>
+  <si>
+    <t>Chairs Produced less DC Chairs Received</t>
+  </si>
+  <si>
+    <t>Production  &lt;= Production Capacity</t>
+  </si>
+  <si>
+    <t>Demand Forecast &lt;= Delivered Units (to Customers)</t>
+  </si>
+  <si>
+    <t>-Check Factory active constraint :: does not seem implemented based on DC Inbound results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -424,6 +436,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -600,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -699,6 +718,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2327,7 +2348,7 @@
   <dimension ref="B2:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2593,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="V8" s="24" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="W8" s="24"/>
     </row>
@@ -2797,7 +2818,7 @@
       <c r="I13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="40">
         <v>30000</v>
       </c>
       <c r="K13" s="2">
@@ -3522,7 +3543,7 @@
         <v>130000</v>
       </c>
       <c r="T35" s="31" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="U35" s="32"/>
       <c r="V35" s="32"/>
@@ -3547,7 +3568,7 @@
         <v>4</v>
       </c>
       <c r="T37" s="31" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="U37" s="32"/>
       <c r="V37" s="32"/>
@@ -3569,6 +3590,9 @@
       <c r="W38" s="33"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C39" s="41" t="s">
+        <v>102</v>
+      </c>
       <c r="N39" s="1" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
improved adv-distribution-good.xlsx and displayed model outcomes for the python vresion
</commit_message>
<xml_diff>
--- a/excel/adv-distribution-goods.xlsx
+++ b/excel/adv-distribution-goods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejwda\Google Drive\01-ejw-data-github\Public\Algorithms\algo-linear-programming\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E48B90-4864-496A-B74F-91B2628F6C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F35D61D-4A31-4EB1-838C-F16A44499639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1170" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{892D736E-9111-411A-81B5-8617378C0CEA}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Executed_Solver!$I$4:$K$5</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">Executed_Solver!$O$4:$Q$5</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">Executed_Solver!$O$9:$Q$10</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Executed_Solver!$U$4:$U$19</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Executed_Solver!$U$4:$U$25</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
@@ -36,7 +36,7 @@
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">Executed_Solver!$U$23</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Executed_Solver!$U$29</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="112">
   <si>
     <t>Beds</t>
   </si>
@@ -411,14 +411,45 @@
     <t>Demand Forecast &lt;= Delivered Units (to Customers)</t>
   </si>
   <si>
-    <t>-Check Factory active constraint :: does not seem implemented based on DC Inbound results</t>
+    <t>Factory1 Tables less DC Inbound Factory1 Tables</t>
+  </si>
+  <si>
+    <t>Factory1 Beds less DC Inbound Factory1 Beds</t>
+  </si>
+  <si>
+    <t>Factory2 Chairs less DC Inbound Factory2 Chairs</t>
+  </si>
+  <si>
+    <t>Factory2 Tables less DC Inbound Factory2 Tables</t>
+  </si>
+  <si>
+    <t>Factory2 Beds less DC Inbound Factory2 Beds</t>
+  </si>
+  <si>
+    <t>Factory1 Chairs less DC Inbound Factory1 Chairs</t>
+  </si>
+  <si>
+    <t>Factory Transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes:  </t>
+  </si>
+  <si>
+    <t>Added the Factory Transfer constraints since the Production Table and DC Inbound table did not agree</t>
+  </si>
+  <si>
+    <t>Not sure if the distribution between production and DC Inbound Tables makes sense</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -443,6 +474,19 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -616,10 +660,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -672,25 +717,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -698,6 +726,15 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -709,19 +746,39 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1116,10 +1173,10 @@
       <c r="U3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="25" t="s">
+      <c r="V3" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="W3" s="26"/>
+      <c r="W3" s="40"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -1156,10 +1213,10 @@
         <f>O15-O17</f>
         <v>0</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="W4" s="24"/>
+      <c r="W4" s="41"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -1196,10 +1253,10 @@
         <f>O16-O18</f>
         <v>0</v>
       </c>
-      <c r="V5" s="24" t="s">
+      <c r="V5" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="W5" s="24"/>
+      <c r="W5" s="41"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -1224,10 +1281,10 @@
         <f>O19-O21</f>
         <v>0</v>
       </c>
-      <c r="V6" s="24" t="s">
+      <c r="V6" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="W6" s="24"/>
+      <c r="W6" s="41"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -1255,10 +1312,10 @@
         <f>O20-O22</f>
         <v>0</v>
       </c>
-      <c r="V7" s="24" t="s">
+      <c r="V7" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="W7" s="24"/>
+      <c r="W7" s="41"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N8" s="6" t="s">
@@ -1280,10 +1337,10 @@
         <f t="shared" ref="U8:U13" si="0">O26-O29</f>
         <v>0</v>
       </c>
-      <c r="V8" s="24" t="s">
+      <c r="V8" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="W8" s="24"/>
+      <c r="W8" s="41"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -1314,10 +1371,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V9" s="24" t="s">
+      <c r="V9" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="W9" s="24"/>
+      <c r="W9" s="41"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -1372,10 +1429,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V10" s="24" t="s">
+      <c r="V10" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="W10" s="24"/>
+      <c r="W10" s="41"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -1409,10 +1466,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V11" s="24" t="s">
+      <c r="V11" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="W11" s="24"/>
+      <c r="W11" s="41"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -1446,10 +1503,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V12" s="24" t="s">
+      <c r="V12" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="W12" s="24"/>
+      <c r="W12" s="41"/>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -1486,10 +1543,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V13" s="24" t="s">
+      <c r="V13" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="W13" s="24"/>
+      <c r="W13" s="41"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -1529,10 +1586,10 @@
         <f t="shared" ref="U14:U19" si="2">O38-O44</f>
         <v>0</v>
       </c>
-      <c r="V14" s="24" t="s">
+      <c r="V14" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="W14" s="24"/>
+      <c r="W14" s="41"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N15" s="1" t="s">
@@ -1549,10 +1606,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V15" s="24" t="s">
+      <c r="V15" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="W15" s="24"/>
+      <c r="W15" s="41"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
@@ -1575,10 +1632,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V16" s="24" t="s">
+      <c r="V16" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="W16" s="24"/>
+      <c r="W16" s="41"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -1625,10 +1682,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V17" s="24" t="s">
+      <c r="V17" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="W17" s="24"/>
+      <c r="W17" s="41"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -1669,10 +1726,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V18" s="24" t="s">
+      <c r="V18" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="W18" s="24"/>
+      <c r="W18" s="41"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -1713,10 +1770,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V19" s="24" t="s">
+      <c r="V19" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="W19" s="24"/>
+      <c r="W19" s="41"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
@@ -1750,8 +1807,8 @@
         <f>SUM(J12:L12)+SUM(J14:L14)</f>
         <v>0</v>
       </c>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
+      <c r="V20" s="38"/>
+      <c r="W20" s="38"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
@@ -1919,12 +1976,12 @@
         <f>SUM(J4:J5)</f>
         <v>0</v>
       </c>
-      <c r="T27" s="28" t="s">
+      <c r="T27" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="U27" s="29"/>
-      <c r="V27" s="29"/>
-      <c r="W27" s="30"/>
+      <c r="U27" s="36"/>
+      <c r="V27" s="36"/>
+      <c r="W27" s="37"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
@@ -1961,12 +2018,12 @@
         <f>SUM(K4:K5)</f>
         <v>0</v>
       </c>
-      <c r="T28" s="31" t="s">
+      <c r="T28" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="U28" s="32"/>
-      <c r="V28" s="32"/>
-      <c r="W28" s="33"/>
+      <c r="U28" s="27"/>
+      <c r="V28" s="27"/>
+      <c r="W28" s="28"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
@@ -2003,10 +2060,10 @@
         <f>SUM(J11:J14)</f>
         <v>0</v>
       </c>
-      <c r="T29" s="34"/>
-      <c r="U29" s="35"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="36"/>
+      <c r="T29" s="32"/>
+      <c r="U29" s="33"/>
+      <c r="V29" s="33"/>
+      <c r="W29" s="34"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
@@ -2058,12 +2115,12 @@
         <f>SUM(L11:L14)</f>
         <v>0</v>
       </c>
-      <c r="T31" s="31" t="s">
+      <c r="T31" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="U31" s="32"/>
-      <c r="V31" s="32"/>
-      <c r="W31" s="33"/>
+      <c r="U31" s="27"/>
+      <c r="V31" s="27"/>
+      <c r="W31" s="28"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
@@ -2076,10 +2133,10 @@
         <f>SUM(J18:J23)</f>
         <v>0</v>
       </c>
-      <c r="T32" s="34"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="36"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="33"/>
+      <c r="V32" s="33"/>
+      <c r="W32" s="34"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
@@ -2102,12 +2159,12 @@
         <f>SUM(K18:K23)</f>
         <v>0</v>
       </c>
-      <c r="T33" s="28" t="s">
+      <c r="T33" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="U33" s="29"/>
-      <c r="V33" s="29"/>
-      <c r="W33" s="30"/>
+      <c r="U33" s="36"/>
+      <c r="V33" s="36"/>
+      <c r="W33" s="37"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
@@ -2129,12 +2186,12 @@
         <f>SUM(L18:L23)</f>
         <v>0</v>
       </c>
-      <c r="T34" s="31" t="s">
+      <c r="T34" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="U34" s="32"/>
-      <c r="V34" s="32"/>
-      <c r="W34" s="33"/>
+      <c r="U34" s="27"/>
+      <c r="V34" s="27"/>
+      <c r="W34" s="28"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
@@ -2149,23 +2206,23 @@
       <c r="E35" s="9">
         <v>130000</v>
       </c>
-      <c r="T35" s="31" t="s">
+      <c r="T35" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="U35" s="32"/>
-      <c r="V35" s="32"/>
-      <c r="W35" s="33"/>
+      <c r="U35" s="27"/>
+      <c r="V35" s="27"/>
+      <c r="W35" s="28"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N36" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="T36" s="31" t="s">
+      <c r="T36" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="U36" s="32"/>
-      <c r="V36" s="32"/>
-      <c r="W36" s="33"/>
+      <c r="U36" s="27"/>
+      <c r="V36" s="27"/>
+      <c r="W36" s="28"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N37" s="1" t="s">
@@ -2174,12 +2231,12 @@
       <c r="O37" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="T37" s="31" t="s">
+      <c r="T37" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="U37" s="32"/>
-      <c r="V37" s="32"/>
-      <c r="W37" s="33"/>
+      <c r="U37" s="27"/>
+      <c r="V37" s="27"/>
+      <c r="W37" s="28"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N38" s="1" t="s">
@@ -2189,12 +2246,12 @@
         <f>J11+J13</f>
         <v>0</v>
       </c>
-      <c r="T38" s="31" t="s">
+      <c r="T38" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="U38" s="32"/>
-      <c r="V38" s="32"/>
-      <c r="W38" s="33"/>
+      <c r="U38" s="27"/>
+      <c r="V38" s="27"/>
+      <c r="W38" s="28"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N39" s="1" t="s">
@@ -2217,10 +2274,10 @@
         <f>L11+L13</f>
         <v>0</v>
       </c>
-      <c r="T40" s="37"/>
-      <c r="U40" s="38"/>
-      <c r="V40" s="38"/>
-      <c r="W40" s="39"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="30"/>
+      <c r="V40" s="30"/>
+      <c r="W40" s="31"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N41" s="1" t="s">
@@ -2306,19 +2363,12 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="T38:W38"/>
-    <mergeCell ref="T40:W40"/>
-    <mergeCell ref="T32:W32"/>
-    <mergeCell ref="T33:W33"/>
-    <mergeCell ref="T34:W34"/>
-    <mergeCell ref="T35:W35"/>
-    <mergeCell ref="T36:W36"/>
-    <mergeCell ref="T37:W37"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="T27:W27"/>
-    <mergeCell ref="T28:W28"/>
-    <mergeCell ref="T29:W29"/>
-    <mergeCell ref="T31:W31"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="V12:W12"/>
+    <mergeCell ref="V13:W13"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="V14:W14"/>
     <mergeCell ref="V15:W15"/>
@@ -2330,12 +2380,19 @@
     <mergeCell ref="V7:W7"/>
     <mergeCell ref="V8:W8"/>
     <mergeCell ref="V9:W9"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="V12:W12"/>
-    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="T27:W27"/>
+    <mergeCell ref="T28:W28"/>
+    <mergeCell ref="T29:W29"/>
+    <mergeCell ref="T31:W31"/>
+    <mergeCell ref="T38:W38"/>
+    <mergeCell ref="T40:W40"/>
+    <mergeCell ref="T32:W32"/>
+    <mergeCell ref="T33:W33"/>
+    <mergeCell ref="T34:W34"/>
+    <mergeCell ref="T35:W35"/>
+    <mergeCell ref="T36:W36"/>
+    <mergeCell ref="T37:W37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2345,10 +2402,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6190072-4778-451D-9493-5F57373D95C5}">
-  <dimension ref="B2:W49"/>
+  <dimension ref="B2:W53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2410,13 +2467,13 @@
       <c r="N3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="T3" s="1" t="s">
@@ -2425,10 +2482,10 @@
       <c r="U3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="25" t="s">
+      <c r="V3" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="W3" s="26"/>
+      <c r="W3" s="40"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -2477,10 +2534,10 @@
         <f>O15-O17</f>
         <v>0</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="W4" s="24"/>
+      <c r="W4" s="41"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2505,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="9">
-        <v>70000.000000000015</v>
+        <v>70000.000000000029</v>
       </c>
       <c r="K5" s="9">
         <v>130000</v>
@@ -2529,10 +2586,10 @@
         <f>O16-O18</f>
         <v>0</v>
       </c>
-      <c r="V5" s="24" t="s">
+      <c r="V5" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="W5" s="24"/>
+      <c r="W5" s="41"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -2557,10 +2614,10 @@
         <f>O19-O21</f>
         <v>0</v>
       </c>
-      <c r="V6" s="24" t="s">
+      <c r="V6" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="W6" s="24"/>
+      <c r="W6" s="41"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -2588,35 +2645,35 @@
         <f>O20-O22</f>
         <v>0</v>
       </c>
-      <c r="V7" s="24" t="s">
+      <c r="V7" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="W7" s="24"/>
+      <c r="W7" s="41"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="P8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="Q8" s="11" t="s">
+      <c r="Q8" s="14" t="s">
         <v>0</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>57</v>
       </c>
       <c r="U8" s="9">
-        <f t="shared" ref="U8:U13" si="0">O26-O29</f>
-        <v>0</v>
-      </c>
-      <c r="V8" s="24" t="s">
+        <f>O26-O29</f>
+        <v>0</v>
+      </c>
+      <c r="V8" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="W8" s="24"/>
+      <c r="W8" s="42"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -2633,7 +2690,7 @@
         <v>-8000</v>
       </c>
       <c r="P9" s="9">
-        <f t="shared" ref="P9" si="1">J4 - (P4*D34)</f>
+        <f t="shared" ref="P9" si="0">J4 - (P4*D34)</f>
         <v>0</v>
       </c>
       <c r="Q9" s="9">
@@ -2644,13 +2701,13 @@
         <v>57</v>
       </c>
       <c r="U9" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V9" s="24" t="s">
+        <f t="shared" ref="U8:U13" si="1">O27-O30</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="W9" s="24"/>
+      <c r="W9" s="42"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -2692,7 +2749,7 @@
       </c>
       <c r="P10" s="9">
         <f t="shared" ref="P10:Q10" si="2">J5 - (P5*D35)</f>
-        <v>-29999.999999999985</v>
+        <v>-29999.999999999971</v>
       </c>
       <c r="Q10" s="9">
         <f t="shared" si="2"/>
@@ -2702,13 +2759,13 @@
         <v>57</v>
       </c>
       <c r="U10" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V10" s="24" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V10" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="W10" s="24"/>
+      <c r="W10" s="42"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -2739,19 +2796,19 @@
         <v>0</v>
       </c>
       <c r="L11" s="2">
-        <v>109999.99999999999</v>
+        <v>90000</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>57</v>
       </c>
       <c r="U11" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V11" s="24" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="W11" s="24"/>
+      <c r="W11" s="41"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -2776,10 +2833,10 @@
         <v>6</v>
       </c>
       <c r="J12" s="2">
-        <v>62000</v>
-      </c>
-      <c r="K12" s="2">
-        <v>110000.00000000001</v>
+        <v>92000</v>
+      </c>
+      <c r="K12" s="24">
+        <v>99999.999999999985</v>
       </c>
       <c r="L12" s="2">
         <v>40000</v>
@@ -2788,13 +2845,13 @@
         <v>57</v>
       </c>
       <c r="U12" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V12" s="24" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V12" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="W12" s="24"/>
+      <c r="W12" s="41"/>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -2818,14 +2875,14 @@
       <c r="I13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="40">
-        <v>30000</v>
-      </c>
-      <c r="K13" s="2">
-        <v>60000</v>
+      <c r="J13" s="45">
+        <v>0</v>
+      </c>
+      <c r="K13" s="24">
+        <v>70000.000000000029</v>
       </c>
       <c r="L13" s="2">
-        <v>109999.99999999999</v>
+        <v>130000</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>66</v>
@@ -2834,13 +2891,13 @@
         <v>57</v>
       </c>
       <c r="U13" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V13" s="24" t="s">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V13" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="W13" s="24"/>
+      <c r="W13" s="41"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -2886,10 +2943,10 @@
         <f t="shared" ref="U14:U19" si="3">O38-O44</f>
         <v>0</v>
       </c>
-      <c r="V14" s="24" t="s">
+      <c r="V14" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="W14" s="24"/>
+      <c r="W14" s="41"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N15" s="1" t="s">
@@ -2906,10 +2963,10 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V15" s="24" t="s">
+      <c r="V15" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="W15" s="24"/>
+      <c r="W15" s="41"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
@@ -2923,7 +2980,7 @@
       </c>
       <c r="O16" s="11">
         <f>SUM(I5:K5)</f>
-        <v>200000</v>
+        <v>200000.00000000003</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>75</v>
@@ -2932,10 +2989,10 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V16" s="24" t="s">
+      <c r="V16" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="W16" s="24"/>
+      <c r="W16" s="41"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -2982,10 +3039,10 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V17" s="24" t="s">
+      <c r="V17" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="W17" s="24"/>
+      <c r="W17" s="41"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -3023,7 +3080,7 @@
       </c>
       <c r="O18" s="11">
         <f>SUM(J13:L14)</f>
-        <v>200000</v>
+        <v>200000.00000000003</v>
       </c>
       <c r="T18" s="1" t="s">
         <v>75</v>
@@ -3032,10 +3089,10 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V18" s="24" t="s">
+      <c r="V18" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="W18" s="24"/>
+      <c r="W18" s="41"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -3073,19 +3130,19 @@
       </c>
       <c r="O19" s="11" cm="1">
         <f t="array" ref="O19">SUM(J11:L11+J13:L13)</f>
-        <v>310000</v>
+        <v>290000</v>
       </c>
       <c r="T19" s="1" t="s">
         <v>75</v>
       </c>
       <c r="U19" s="9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="V19" s="24" t="s">
+        <f>O43-O49</f>
+        <v>0</v>
+      </c>
+      <c r="V19" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="W19" s="24"/>
+      <c r="W19" s="41"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
@@ -3113,7 +3170,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="2">
-        <v>0</v>
+        <v>10000.000000000015</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>
@@ -3123,10 +3180,19 @@
       </c>
       <c r="O20" s="11">
         <f>SUM(J12:L12)+SUM(J14:L14)</f>
-        <v>212000</v>
-      </c>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
+        <v>232000</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="U20" s="9">
+        <f>I4-SUM(J11:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="V20" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="W20" s="43"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
@@ -3154,18 +3220,29 @@
         <v>12000</v>
       </c>
       <c r="K21" s="2">
-        <v>80000.000000000015</v>
+        <v>69999.999999999985</v>
       </c>
       <c r="L21" s="2">
-        <v>39999.999999999993</v>
+        <v>40000</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>41</v>
       </c>
       <c r="O21" s="11">
         <f>SUM(J18:L18)+SUM(J20:L20)+SUM(J22:L22)</f>
-        <v>310000</v>
-      </c>
+        <v>290000</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="U21" s="9">
+        <f>J4-SUM(K11:K12)</f>
+        <v>0</v>
+      </c>
+      <c r="V21" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="W21" s="43"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
@@ -3190,7 +3267,7 @@
         <v>7</v>
       </c>
       <c r="J22" s="2">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="K22" s="2">
         <v>60000</v>
@@ -3203,11 +3280,19 @@
       </c>
       <c r="O22" s="11">
         <f>SUM(J19:L19)+SUM(J21:L21)+SUM(J23:L23)</f>
-        <v>212000</v>
-      </c>
-      <c r="T22" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>232000</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="U22" s="9">
+        <f>K4-SUM(L11:L12)</f>
+        <v>0</v>
+      </c>
+      <c r="V22" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="W22" s="43"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
@@ -3232,7 +3317,7 @@
         <v>6</v>
       </c>
       <c r="J23" s="2">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="K23" s="2">
         <v>0</v>
@@ -3241,25 +3326,51 @@
         <v>0</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U23" s="8">
-        <f>SUMPRODUCT(D4:F4,I4:K4)+SUMPRODUCT(D6:F6,I5:K5)+SUMPRODUCT(D5:F5,O4:Q4)+SUMPRODUCT(D7:F7,O5:Q5)+SUMPRODUCT(D11:F14,J11:L14)+SUMPRODUCT(D18:F23,J18:L23)</f>
-        <v>44421000</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="U23" s="9">
+        <f>I5-SUM(J13:J14)</f>
+        <v>0</v>
+      </c>
+      <c r="V23" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="W23" s="43"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N24" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="U24" s="9">
+        <f>J5-SUM(K13:K14)</f>
+        <v>0</v>
+      </c>
+      <c r="V24" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="W24" s="43"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O25" s="14" t="s">
         <v>4</v>
       </c>
+      <c r="T25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="U25" s="9">
+        <f>K5-SUM(L13:L14)</f>
+        <v>0</v>
+      </c>
+      <c r="V25" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="W25" s="43"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
@@ -3275,34 +3386,30 @@
         <f>SUM(I4:I5)</f>
         <v>92000</v>
       </c>
-      <c r="T26" s="21"/>
-      <c r="U26" s="22"/>
-      <c r="V26" s="22"/>
-      <c r="W26" s="23"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K27" s="11" t="s">
+      <c r="K27" s="14" t="s">
         <v>0</v>
       </c>
       <c r="N27" s="1" t="s">
@@ -3312,12 +3419,6 @@
         <f>SUM(J4:J5)</f>
         <v>170000</v>
       </c>
-      <c r="T27" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="U27" s="29"/>
-      <c r="V27" s="29"/>
-      <c r="W27" s="30"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
@@ -3354,12 +3455,9 @@
         <f>SUM(K4:K5)</f>
         <v>260000</v>
       </c>
-      <c r="T28" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="U28" s="32"/>
-      <c r="V28" s="32"/>
-      <c r="W28" s="33"/>
+      <c r="T28" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
@@ -3383,11 +3481,11 @@
       </c>
       <c r="J29" s="9">
         <f t="shared" ref="J29:K29" si="5">SUM(K20:K21)</f>
-        <v>80000.000000000015</v>
+        <v>80000</v>
       </c>
       <c r="K29" s="9">
         <f t="shared" si="5"/>
-        <v>39999.999999999993</v>
+        <v>40000</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>50</v>
@@ -3396,10 +3494,13 @@
         <f>SUM(J11:J14)</f>
         <v>92000</v>
       </c>
-      <c r="T29" s="34"/>
-      <c r="U29" s="35"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="36"/>
+      <c r="T29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U29" s="44">
+        <f>SUMPRODUCT(D4:F4,I4:K4)+SUMPRODUCT(D6:F6,I5:K5)+SUMPRODUCT(D5:F5,O4:Q4)+SUMPRODUCT(D7:F7,O5:Q5)+SUMPRODUCT(D11:F14,J11:L14)+SUMPRODUCT(D18:F23,J18:L23)</f>
+        <v>44491000</v>
+      </c>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
@@ -3436,14 +3537,8 @@
         <f>SUM(K11:K14)</f>
         <v>170000</v>
       </c>
-      <c r="T30" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="U30" s="15"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="16"/>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N31" s="1" t="s">
         <v>52</v>
       </c>
@@ -3451,12 +3546,6 @@
         <f>SUM(L11:L14)</f>
         <v>260000</v>
       </c>
-      <c r="T31" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="U31" s="32"/>
-      <c r="V31" s="32"/>
-      <c r="W31" s="33"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
@@ -3469,10 +3558,10 @@
         <f>SUM(J18:J23)</f>
         <v>92000</v>
       </c>
-      <c r="T32" s="34"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="36"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="22"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="23"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
@@ -3495,12 +3584,12 @@
         <f>SUM(K18:K23)</f>
         <v>170000</v>
       </c>
-      <c r="T33" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="U33" s="29"/>
-      <c r="V33" s="29"/>
-      <c r="W33" s="30"/>
+      <c r="T33" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="U33" s="36"/>
+      <c r="V33" s="36"/>
+      <c r="W33" s="37"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
@@ -3522,12 +3611,12 @@
         <f>SUM(L18:L23)</f>
         <v>260000</v>
       </c>
-      <c r="T34" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="U34" s="32"/>
-      <c r="V34" s="32"/>
-      <c r="W34" s="33"/>
+      <c r="T34" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="U34" s="27"/>
+      <c r="V34" s="27"/>
+      <c r="W34" s="28"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
@@ -3542,23 +3631,21 @@
       <c r="E35" s="9">
         <v>130000</v>
       </c>
-      <c r="T35" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="U35" s="32"/>
-      <c r="V35" s="32"/>
-      <c r="W35" s="33"/>
+      <c r="T35" s="32"/>
+      <c r="U35" s="33"/>
+      <c r="V35" s="33"/>
+      <c r="W35" s="34"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N36" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="T36" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="U36" s="32"/>
-      <c r="V36" s="32"/>
-      <c r="W36" s="33"/>
+      <c r="T36" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="16"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N37" s="1" t="s">
@@ -3567,12 +3654,12 @@
       <c r="O37" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="T37" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="U37" s="32"/>
-      <c r="V37" s="32"/>
-      <c r="W37" s="33"/>
+      <c r="T37" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="U37" s="27"/>
+      <c r="V37" s="27"/>
+      <c r="W37" s="28"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N38" s="1" t="s">
@@ -3580,43 +3667,43 @@
       </c>
       <c r="O38" s="11">
         <f>J11+J13</f>
-        <v>30000</v>
-      </c>
-      <c r="T38" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="U38" s="32"/>
-      <c r="V38" s="32"/>
-      <c r="W38" s="33"/>
+        <v>0</v>
+      </c>
+      <c r="T38" s="32"/>
+      <c r="U38" s="33"/>
+      <c r="V38" s="33"/>
+      <c r="W38" s="34"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C39" s="41" t="s">
-        <v>102</v>
-      </c>
+      <c r="C39" s="25"/>
       <c r="N39" s="1" t="s">
         <v>68</v>
       </c>
       <c r="O39" s="11">
         <f>K11+K13</f>
-        <v>60000</v>
-      </c>
-      <c r="T39" s="18"/>
-      <c r="U39" s="19"/>
-      <c r="V39" s="19"/>
-      <c r="W39" s="20"/>
-    </row>
-    <row r="40" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>70000.000000000029</v>
+      </c>
+      <c r="T39" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="U39" s="36"/>
+      <c r="V39" s="36"/>
+      <c r="W39" s="37"/>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N40" s="1" t="s">
         <v>69</v>
       </c>
       <c r="O40" s="11">
         <f>L11+L13</f>
-        <v>219999.99999999997</v>
-      </c>
-      <c r="T40" s="37"/>
-      <c r="U40" s="38"/>
-      <c r="V40" s="38"/>
-      <c r="W40" s="39"/>
+        <v>220000</v>
+      </c>
+      <c r="T40" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="U40" s="27"/>
+      <c r="V40" s="27"/>
+      <c r="W40" s="28"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N41" s="1" t="s">
@@ -3624,8 +3711,14 @@
       </c>
       <c r="O41" s="11">
         <f>J12+J14</f>
-        <v>62000</v>
-      </c>
+        <v>92000</v>
+      </c>
+      <c r="T41" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="U41" s="27"/>
+      <c r="V41" s="27"/>
+      <c r="W41" s="28"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N42" s="1" t="s">
@@ -3633,9 +3726,14 @@
       </c>
       <c r="O42" s="11">
         <f>K12+K14</f>
-        <v>110000.00000000001</v>
-      </c>
-      <c r="T42" s="4"/>
+        <v>99999.999999999985</v>
+      </c>
+      <c r="T42" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="U42" s="27"/>
+      <c r="V42" s="27"/>
+      <c r="W42" s="28"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N43" s="1" t="s">
@@ -3645,6 +3743,12 @@
         <f>L12+L14</f>
         <v>40000</v>
       </c>
+      <c r="T43" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="U43" s="27"/>
+      <c r="V43" s="27"/>
+      <c r="W43" s="28"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N44" s="1" t="s">
@@ -3652,8 +3756,14 @@
       </c>
       <c r="O44" s="11">
         <f>J18+J20+J22</f>
-        <v>30000</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T44" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="U44" s="27"/>
+      <c r="V44" s="27"/>
+      <c r="W44" s="28"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N45" s="1" t="s">
@@ -3661,10 +3771,14 @@
       </c>
       <c r="O45" s="11">
         <f>K18+K20+K22</f>
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+        <v>70000.000000000015</v>
+      </c>
+      <c r="T45" s="18"/>
+      <c r="U45" s="19"/>
+      <c r="V45" s="19"/>
+      <c r="W45" s="20"/>
+    </row>
+    <row r="46" spans="2:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N46" s="1" t="s">
         <v>77</v>
       </c>
@@ -3672,6 +3786,10 @@
         <f>L18+L20+L22</f>
         <v>220000</v>
       </c>
+      <c r="T46" s="29"/>
+      <c r="U46" s="30"/>
+      <c r="V46" s="30"/>
+      <c r="W46" s="31"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
       <c r="N47" s="1" t="s">
@@ -3679,7 +3797,7 @@
       </c>
       <c r="O47" s="11">
         <f>J19+J21+J23</f>
-        <v>62000</v>
+        <v>92000</v>
       </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
@@ -3688,32 +3806,48 @@
       </c>
       <c r="O48" s="11">
         <f>K19+K21+K23</f>
-        <v>110000.00000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="14:15" x14ac:dyDescent="0.25">
+        <v>99999.999999999985</v>
+      </c>
+      <c r="T48" s="4"/>
+    </row>
+    <row r="49" spans="14:20" x14ac:dyDescent="0.25">
       <c r="N49" s="1" t="s">
         <v>80</v>
       </c>
       <c r="O49" s="11">
         <f>L19+L21+L23</f>
-        <v>39999.999999999993</v>
+        <v>40000</v>
+      </c>
+      <c r="T49" s="46"/>
+    </row>
+    <row r="51" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="T51" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="T52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="T53" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="T40:W40"/>
-    <mergeCell ref="T27:W27"/>
-    <mergeCell ref="T28:W28"/>
-    <mergeCell ref="T29:W29"/>
-    <mergeCell ref="T31:W31"/>
-    <mergeCell ref="T32:W32"/>
-    <mergeCell ref="T33:W33"/>
-    <mergeCell ref="T34:W34"/>
-    <mergeCell ref="T35:W35"/>
-    <mergeCell ref="T36:W36"/>
-    <mergeCell ref="T37:W37"/>
-    <mergeCell ref="T38:W38"/>
+  <mergeCells count="35">
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="V7:W7"/>
     <mergeCell ref="V20:W20"/>
     <mergeCell ref="V9:W9"/>
     <mergeCell ref="V10:W10"/>
@@ -3726,12 +3860,18 @@
     <mergeCell ref="V17:W17"/>
     <mergeCell ref="V18:W18"/>
     <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="T46:W46"/>
+    <mergeCell ref="T33:W33"/>
+    <mergeCell ref="T34:W34"/>
+    <mergeCell ref="T35:W35"/>
+    <mergeCell ref="T37:W37"/>
+    <mergeCell ref="T38:W38"/>
+    <mergeCell ref="T39:W39"/>
+    <mergeCell ref="T40:W40"/>
+    <mergeCell ref="T41:W41"/>
+    <mergeCell ref="T42:W42"/>
+    <mergeCell ref="T43:W43"/>
+    <mergeCell ref="T44:W44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>